<commit_message>
DOM Changes in PROD
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC02_Verify_MYACC_RegisteredUser.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC02_Verify_MYACC_RegisteredUser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7F060D-D48C-4D0A-8042-1CD8E37738BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1472928-CDEC-46CD-9465-E521E52A12E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC02_Verify_MYACC_RegisteredUse" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
   <si>
     <t>TestCase</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>LoginButton</t>
+  </si>
+  <si>
+    <t>PurchasingHistory</t>
+  </si>
+  <si>
+    <t>Purchasing History</t>
+  </si>
+  <si>
+    <t>QuickOrderMyacc</t>
+  </si>
+  <si>
+    <t>Storerooms</t>
   </si>
 </sst>
 </file>
@@ -599,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -859,7 +871,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>50</v>
@@ -874,7 +886,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>50</v>
@@ -889,7 +901,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>50</v>
@@ -952,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1071,7 +1083,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1087,7 +1099,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1180,21 +1192,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1391,24 +1388,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1425,4 +1420,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>